<commit_message>
agregue el trabajo del sabado
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{260D3264-C259-4A8D-83BC-D9F6DAD39B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD4159C-D039-4139-8A3B-3B0AD8C526F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Fecha</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Todo está claro por el momento. Excelente tutorial</t>
+  </si>
+  <si>
+    <t>Css Grid y Flex box (4 horas)</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,8 +565,12 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>117778</v>
+      </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -823,60 +830,18 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -892,18 +857,60 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy 20/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD4159C-D039-4139-8A3B-3B0AD8C526F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966225D4-DCF8-44D1-882D-FD1E837C843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Fecha</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Css Grid y Flex box (4 horas)</t>
+  </si>
+  <si>
+    <t>Terminé el primer proyecto sitio web freelancer</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+      <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,8 +582,12 @@
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7">
+        <v>44732</v>
+      </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -830,18 +837,60 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -857,60 +906,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy 21/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966225D4-DCF8-44D1-882D-FD1E837C843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBBE593-0F0A-4659-B420-796852A4FA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Fecha</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Terminé el primer proyecto sitio web freelancer</t>
+  </si>
+  <si>
+    <t>Inicio proyecto Frontend Store y metodología BEM</t>
   </si>
 </sst>
 </file>
@@ -522,7 +525,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C10"/>
+      <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,8 +599,12 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="7">
+        <v>44733</v>
+      </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -837,60 +844,18 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -906,18 +871,60 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy 22/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBBE593-0F0A-4659-B420-796852A4FA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51311DB0-13F4-4BD1-9F15-2C9D235BBFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Fecha</t>
   </si>
@@ -56,10 +56,13 @@
     <t>Css Grid y Flex box (4 horas)</t>
   </si>
   <si>
-    <t>Terminé el primer proyecto sitio web freelancer</t>
+    <t>Terminé el primer proyecto sitio web freelancer (6 horas)</t>
   </si>
   <si>
-    <t>Inicio proyecto Frontend Store y metodología BEM</t>
+    <t>Inicio proyecto Frontend Store y metodología BEM (6 horas)</t>
+  </si>
+  <si>
+    <t>Terminé el segundo proyecto Frontend Store  (6 horas)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
@@ -613,8 +616,12 @@
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="7">
+        <v>44734</v>
+      </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -844,18 +851,60 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -871,60 +920,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el avance de hoy 23/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51311DB0-13F4-4BD1-9F15-2C9D235BBFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC77EB1-7900-4366-A2AF-3C8D458258DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Fecha</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Terminé el segundo proyecto Frontend Store  (6 horas)</t>
+  </si>
+  <si>
+    <t>Curso de JavaScript moderno variables, Strings, números, Operadores (6 horas)</t>
   </si>
 </sst>
 </file>
@@ -527,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,8 +633,12 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="7">
+        <v>44735</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -851,60 +858,18 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -920,18 +885,60 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy 24/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC77EB1-7900-4366-A2AF-3C8D458258DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438449D-0E16-4C6D-B4C7-2DD572698FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Curso de JavaScript moderno variables, Strings, números, Operadores (6 horas)</t>
+  </si>
+  <si>
+    <t>Curso de JavaScript moderno Booleanos, operadores y funciones (6 horas)</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,8 +650,12 @@
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="7">
+        <v>44736</v>
+      </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -858,18 +865,60 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -885,60 +934,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue trabajo de hoy 27/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438449D-0E16-4C6D-B4C7-2DD572698FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C664014-1C69-42BF-921F-8F0D6F0662DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Fecha</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Curso de JavaScript moderno Booleanos, operadores y funciones (6 horas)</t>
+  </si>
+  <si>
+    <t>Curso de JavaScript  Objectos y Arrays(6 horas)</t>
   </si>
 </sst>
 </file>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,8 +667,12 @@
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="7">
+        <v>44739</v>
+      </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -865,60 +872,18 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -934,18 +899,60 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy 28/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C664014-1C69-42BF-921F-8F0D6F0662DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3387EC2A-ED34-4086-93DA-16E3DFB6A325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Fecha</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Curso de JavaScript  Objectos y Arrays(6 horas)</t>
+  </si>
+  <si>
+    <t>Curso de JavaScript moderno ciclo while, do while, for, Swich, if else , if anidados.</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+      <selection activeCell="D21" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,8 +684,12 @@
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="7">
+        <v>44740</v>
+      </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -872,18 +879,60 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -899,60 +948,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy 29/6/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3387EC2A-ED34-4086-93DA-16E3DFB6A325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5664D9-8D18-4CF6-967F-3371D30465DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Fecha</t>
   </si>
@@ -71,10 +71,13 @@
     <t>Curso de JavaScript moderno Booleanos, operadores y funciones (6 horas)</t>
   </si>
   <si>
-    <t>Curso de JavaScript  Objectos y Arrays(6 horas)</t>
-  </si>
-  <si>
     <t>Curso de JavaScript moderno ciclo while, do while, for, Swich, if else , if anidados.</t>
+  </si>
+  <si>
+    <t>Curso de JavaScript  Objetos y Arrays(6 horas)</t>
+  </si>
+  <si>
+    <t>Curso de JavaScript moderno funciones, Estructuras de control e iteradores</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +674,7 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="7">
         <v>44739</v>
@@ -685,7 +688,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="7">
         <v>44740</v>
@@ -698,8 +701,12 @@
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="7">
+        <v>44741</v>
+      </c>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -879,60 +886,18 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -948,18 +913,60 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5664D9-8D18-4CF6-967F-3371D30465DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE58BF6-3450-4033-B132-2B2B0AC22766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Fecha</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Curso de JavaScript moderno funciones, Estructuras de control e iteradores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curso de JavaScript moderno ,Array Methods,Dom, eventos </t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D28"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,8 +718,12 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="7">
+        <v>44742</v>
+      </c>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -886,18 +893,60 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -913,60 +962,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue la practica de hoy 1/7/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE58BF6-3450-4033-B132-2B2B0AC22766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2783AAEB-ACC5-4810-BDBB-3841C66C2E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Fecha</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">Curso de JavaScript moderno ,Array Methods,Dom, eventos </t>
+  </si>
+  <si>
+    <t>Práctica de JavaScript en el navegator y Dom scripting</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E27" sqref="E27:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,8 +735,12 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="7">
+        <v>44743</v>
+      </c>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -893,60 +900,18 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -962,18 +927,60 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el trabajo de hoy 4/7/2022
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2783AAEB-ACC5-4810-BDBB-3841C66C2E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A534F16-7C25-4EB9-A66E-BE42A0819719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Fecha</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Práctica de JavaScript en el navegator y Dom scripting</t>
+  </si>
+  <si>
+    <t>Curso de Gulp y Saas</t>
   </si>
 </sst>
 </file>
@@ -548,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:E28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,8 +752,12 @@
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="7">
+        <v>44746</v>
+      </c>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -900,18 +907,60 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -927,60 +976,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue los temas  revisados
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A534F16-7C25-4EB9-A66E-BE42A0819719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E96FBE-F37E-4B8A-83BF-4C3B2E4F96BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Fecha</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Curso de Gulp y Saas</t>
+  </si>
+  <si>
+    <t>Temas aprendidos: Poo, Prototypes, clase, herencia y Try Catch</t>
+  </si>
+  <si>
+    <t>Temas aprendidos:  Async Await, Fetch Api , introducción a Php</t>
   </si>
 </sst>
 </file>
@@ -551,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:D30"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,8 +772,12 @@
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="7">
+        <v>44747</v>
+      </c>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -776,8 +786,12 @@
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="7">
+        <v>44748</v>
+      </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -907,60 +921,18 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -976,18 +948,60 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregue el aprendizaje de hoy
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\GitHub\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E96FBE-F37E-4B8A-83BF-4C3B2E4F96BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF9F8A9-085D-4B93-931B-48DEC7A06E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Fecha</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Temas aprendidos:  Async Await, Fetch Api , introducción a Php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temas aprendidos: SQL CRUD </t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C30"/>
+      <selection activeCell="E33" sqref="E33:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,8 +803,12 @@
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="7">
+        <v>44749</v>
+      </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -921,18 +928,60 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -948,60 +997,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>